<commit_message>
Previsoes e numeros atualizados 29/03/2019
</commit_message>
<xml_diff>
--- a/LEC_EUROPA_2019.xlsx
+++ b/LEC_EUROPA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3E84B2-F87D-40B7-9CF1-EE2AA8220FD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957B0B28-E188-44F4-8EB8-37F114B9C333}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="155">
   <si>
     <t>Lanes</t>
   </si>
@@ -1552,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C7BB09-4029-452F-B902-3394B5983D34}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2570,6 +2570,39 @@
       </c>
       <c r="C92" s="82">
         <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C94" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C95" s="80">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>